<commit_message>
Add updated fatigueRepReport and MATLAB ppt
</commit_message>
<xml_diff>
--- a/Capstone/data/results/fatigueRepReport.xlsx
+++ b/Capstone/data/results/fatigueRepReport.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="16828"/>
-  <workbookPr defaultThemeVersion="164011"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Todd\Documents\GitHub\SHAF\Capstone\data\results\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="N:\SHAF\Capstone\data\results\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1072,7 +1072,7 @@
   <dimension ref="A1:D17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G18" sqref="G18"/>
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1100,13 +1100,13 @@
         <v>0.1</v>
       </c>
       <c r="B2" s="4">
-        <v>1097</v>
+        <v>1816</v>
       </c>
       <c r="C2" s="4">
-        <v>187</v>
+        <v>357</v>
       </c>
       <c r="D2" s="1">
-        <v>-910</v>
+        <v>-1459</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -1114,13 +1114,13 @@
         <v>0.12</v>
       </c>
       <c r="B3" s="5">
-        <v>1097</v>
+        <v>1816</v>
       </c>
       <c r="C3" s="5">
-        <v>204</v>
+        <v>596</v>
       </c>
       <c r="D3" s="2">
-        <v>-893</v>
+        <v>-1220</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
@@ -1128,13 +1128,13 @@
         <v>0.14000000000000001</v>
       </c>
       <c r="B4" s="5">
-        <v>1097</v>
+        <v>1816</v>
       </c>
       <c r="C4" s="5">
-        <v>223</v>
+        <v>615</v>
       </c>
       <c r="D4" s="2">
-        <v>-874</v>
+        <v>-1201</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
@@ -1142,13 +1142,13 @@
         <v>0.16</v>
       </c>
       <c r="B5" s="5">
-        <v>1097</v>
+        <v>1816</v>
       </c>
       <c r="C5" s="5">
-        <v>236</v>
+        <v>720</v>
       </c>
       <c r="D5" s="2">
-        <v>-861</v>
+        <v>-1096</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
@@ -1156,13 +1156,13 @@
         <v>0.18</v>
       </c>
       <c r="B6" s="5">
-        <v>1097</v>
+        <v>1816</v>
       </c>
       <c r="C6" s="5">
-        <v>263</v>
+        <v>692</v>
       </c>
       <c r="D6" s="2">
-        <v>-834</v>
+        <v>-1124</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
@@ -1170,13 +1170,13 @@
         <v>0.2</v>
       </c>
       <c r="B7" s="5">
-        <v>1097</v>
+        <v>1816</v>
       </c>
       <c r="C7" s="5">
-        <v>268</v>
+        <v>517</v>
       </c>
       <c r="D7" s="2">
-        <v>-829</v>
+        <v>-1299</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
@@ -1184,13 +1184,13 @@
         <v>0.22</v>
       </c>
       <c r="B8" s="5">
-        <v>1097</v>
+        <v>1816</v>
       </c>
       <c r="C8" s="5">
         <v>279</v>
       </c>
       <c r="D8" s="2">
-        <v>-818</v>
+        <v>-1537</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
@@ -1198,13 +1198,13 @@
         <v>0.24</v>
       </c>
       <c r="B9" s="5">
-        <v>1097</v>
+        <v>1816</v>
       </c>
       <c r="C9" s="5">
         <v>270</v>
       </c>
       <c r="D9" s="2">
-        <v>-827</v>
+        <v>-1546</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
@@ -1212,13 +1212,13 @@
         <v>0.26</v>
       </c>
       <c r="B10" s="5">
-        <v>1097</v>
+        <v>1816</v>
       </c>
       <c r="C10" s="5">
         <v>277</v>
       </c>
       <c r="D10" s="2">
-        <v>-820</v>
+        <v>-1539</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
@@ -1226,13 +1226,13 @@
         <v>0.28000000000000003</v>
       </c>
       <c r="B11" s="5">
-        <v>1097</v>
+        <v>1816</v>
       </c>
       <c r="C11" s="5">
         <v>290</v>
       </c>
       <c r="D11" s="2">
-        <v>-807</v>
+        <v>-1526</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
@@ -1240,13 +1240,13 @@
         <v>0.3</v>
       </c>
       <c r="B12" s="5">
-        <v>1097</v>
+        <v>1816</v>
       </c>
       <c r="C12" s="5">
         <v>287</v>
       </c>
       <c r="D12" s="2">
-        <v>-810</v>
+        <v>-1529</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
@@ -1254,13 +1254,13 @@
         <v>0.32</v>
       </c>
       <c r="B13" s="5">
-        <v>1097</v>
+        <v>1816</v>
       </c>
       <c r="C13" s="5">
         <v>284</v>
       </c>
       <c r="D13" s="2">
-        <v>-813</v>
+        <v>-1532</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
@@ -1268,13 +1268,13 @@
         <v>0.34</v>
       </c>
       <c r="B14" s="5">
-        <v>1097</v>
+        <v>1816</v>
       </c>
       <c r="C14" s="5">
         <v>272</v>
       </c>
       <c r="D14" s="2">
-        <v>-825</v>
+        <v>-1544</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
@@ -1282,13 +1282,13 @@
         <v>0.36</v>
       </c>
       <c r="B15" s="5">
-        <v>1097</v>
+        <v>1816</v>
       </c>
       <c r="C15" s="5">
         <v>261</v>
       </c>
       <c r="D15" s="2">
-        <v>-836</v>
+        <v>-1555</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
@@ -1296,13 +1296,13 @@
         <v>0.38</v>
       </c>
       <c r="B16" s="5">
-        <v>1097</v>
+        <v>1816</v>
       </c>
       <c r="C16" s="5">
         <v>252</v>
       </c>
       <c r="D16" s="2">
-        <v>-845</v>
+        <v>-1564</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1310,13 +1310,13 @@
         <v>0.4</v>
       </c>
       <c r="B17" s="6">
-        <v>1097</v>
+        <v>1816</v>
       </c>
       <c r="C17" s="6">
         <v>250</v>
       </c>
       <c r="D17" s="3">
-        <v>-847</v>
+        <v>-1566</v>
       </c>
     </row>
   </sheetData>
@@ -1331,6 +1331,6 @@
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>